<commit_message>
update feature notes 1
</commit_message>
<xml_diff>
--- a/Feature_notes_.xlsx
+++ b/Feature_notes_.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joe Fritch\Documents\NYCDSA\Projects\ML_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B70D75-5F95-493A-A3DA-E2766BAA6DDB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819E5594-7741-4534-AB59-B6F4DBEE0580}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3560" yWindow="3180" windowWidth="14400" windowHeight="7360" xr2:uid="{106BEA56-9D90-4FC1-81C5-5AFEC1DAF831}"/>
+    <workbookView xWindow="3560" yWindow="2840" windowWidth="14400" windowHeight="7360" xr2:uid="{106BEA56-9D90-4FC1-81C5-5AFEC1DAF831}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="89">
   <si>
     <t>Id</t>
   </si>
@@ -286,6 +286,18 @@
   </si>
   <si>
     <t>Ordinal</t>
+  </si>
+  <si>
+    <t>Quality has order</t>
+  </si>
+  <si>
+    <t>Condition has order</t>
+  </si>
+  <si>
+    <t>Year has order</t>
+  </si>
+  <si>
+    <t>Remove Row</t>
   </si>
 </sst>
 </file>
@@ -649,7 +661,7 @@
   <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -657,6 +669,7 @@
     <col min="1" max="1" width="13.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.08984375" customWidth="1"/>
+    <col min="4" max="4" width="17.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -680,6 +693,12 @@
       <c r="B2">
         <v>0</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -687,6 +706,9 @@
       </c>
       <c r="B3">
         <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -696,6 +718,9 @@
       <c r="B4">
         <v>1</v>
       </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -704,6 +729,9 @@
       <c r="B5">
         <v>0</v>
       </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -712,6 +740,9 @@
       <c r="B6">
         <v>0</v>
       </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -720,6 +751,9 @@
       <c r="B7">
         <v>1</v>
       </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -728,6 +762,9 @@
       <c r="B8">
         <v>1</v>
       </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -736,6 +773,9 @@
       <c r="B9">
         <v>1</v>
       </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -744,6 +784,9 @@
       <c r="B10">
         <v>1</v>
       </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -752,6 +795,9 @@
       <c r="B11">
         <v>1</v>
       </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -760,6 +806,9 @@
       <c r="B12">
         <v>1</v>
       </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -768,6 +817,9 @@
       <c r="B13">
         <v>1</v>
       </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -776,6 +828,9 @@
       <c r="B14">
         <v>1</v>
       </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -784,6 +839,9 @@
       <c r="B15">
         <v>1</v>
       </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -792,532 +850,778 @@
       <c r="B16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
       <c r="B19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
       <c r="B20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
       <c r="B22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
       <c r="B24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
       <c r="B25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>34</v>
       </c>
       <c r="B36">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>35</v>
       </c>
       <c r="B37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>36</v>
       </c>
       <c r="B38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>37</v>
       </c>
       <c r="B39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>38</v>
       </c>
       <c r="B40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>39</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>40</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>41</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>42</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>43</v>
       </c>
       <c r="B45">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>44</v>
       </c>
       <c r="B46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>45</v>
       </c>
       <c r="B47">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>46</v>
       </c>
       <c r="B48">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>47</v>
       </c>
       <c r="B49">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>48</v>
       </c>
       <c r="B50">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>49</v>
       </c>
       <c r="B51">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>50</v>
       </c>
       <c r="B52">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>51</v>
       </c>
       <c r="B53">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>52</v>
       </c>
       <c r="B54">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>53</v>
       </c>
       <c r="B55">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C55">
+        <v>1</v>
+      </c>
+      <c r="D55" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>54</v>
       </c>
       <c r="B56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>55</v>
       </c>
       <c r="B57">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>56</v>
       </c>
       <c r="B58">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>57</v>
       </c>
       <c r="B59">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>58</v>
       </c>
       <c r="B60">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>59</v>
       </c>
       <c r="B61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>60</v>
       </c>
       <c r="B62">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>61</v>
       </c>
       <c r="B63">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>62</v>
       </c>
       <c r="B64">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>63</v>
       </c>
       <c r="B65">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C65">
+        <v>1</v>
+      </c>
+      <c r="D65" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>64</v>
       </c>
       <c r="B66">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C66">
+        <v>1</v>
+      </c>
+      <c r="D66" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>65</v>
       </c>
       <c r="B67">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>66</v>
       </c>
       <c r="B68">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>67</v>
       </c>
       <c r="B69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>68</v>
       </c>
       <c r="B70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>69</v>
       </c>
       <c r="B71">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>70</v>
       </c>
       <c r="B72">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>71</v>
       </c>
       <c r="B73">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>72</v>
       </c>
       <c r="B74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>73</v>
       </c>
       <c r="B75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>74</v>
       </c>
       <c r="B76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>75</v>
       </c>
       <c r="B77">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>76</v>
       </c>
       <c r="B78">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>77</v>
       </c>
       <c r="B79">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>78</v>
       </c>
       <c r="B80">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>79</v>
       </c>
       <c r="B81">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>80</v>
       </c>
       <c r="B82">
+        <v>0</v>
+      </c>
+      <c r="C82">
         <v>0</v>
       </c>
     </row>

</xml_diff>